<commit_message>
changes related to web resources folder
</commit_message>
<xml_diff>
--- a/CRM Solution Manager/Release/AzureFunction/AzureKeyVaultNames.xlsx
+++ b/CRM Solution Manager/Release/AzureFunction/AzureKeyVaultNames.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m-ynaresh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m-ynaresh\Downloads\BuildRelase\changes\25112019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8167FECA-DF8B-436B-9DD6-A6EB39323ACC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CCED74-CBEA-42F0-BF6F-816A749DE1FF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{954886C5-4D1A-4ACB-BA8C-D15138D5C5AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Key-Vault secrets" sheetId="2" r:id="rId2"/>
+    <sheet name="Configuration settings" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="85">
   <si>
     <t>ClientApplicationSecret</t>
   </si>
@@ -272,6 +273,108 @@
   <si>
     <t xml:space="preserve">if it is TFS Source control then enter TFS user name and password or enter github user name and password </t>
   </si>
+  <si>
+    <t>https://igdcicd2.crm8.dynamics.com</t>
+  </si>
+  <si>
+    <t>Configuration Key</t>
+  </si>
+  <si>
+    <t>BranchName</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>CloneRepositoryAlways</t>
+  </si>
+  <si>
+    <t>MultilpleSolutionsImport</t>
+  </si>
+  <si>
+    <t>DD365\MultilpleSolutionsImport.ps1</t>
+  </si>
+  <si>
+    <t>RemoteName</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>RepositoryHtmlDirectory</t>
+  </si>
+  <si>
+    <t>RepositoryImagesDirectory</t>
+  </si>
+  <si>
+    <t>RepositoryJsDirectory</t>
+  </si>
+  <si>
+    <t>RepositoryLocalDirectory</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>RepositorySolutionFolder</t>
+  </si>
+  <si>
+    <t>RepositoryUrl</t>
+  </si>
+  <si>
+    <t>https://ReachHigh@dev.azure.com/ReachHigh/DD365/_git/DD365</t>
+  </si>
+  <si>
+    <t>SleepTimeoutInMillis</t>
+  </si>
+  <si>
+    <t>SolutionFile</t>
+  </si>
+  <si>
+    <t>SolutionFileRelease</t>
+  </si>
+  <si>
+    <t>SolutionPackagerPath</t>
+  </si>
+  <si>
+    <t>E:\tools\Tools\CoreTools\solutionpackager.exe</t>
+  </si>
+  <si>
+    <t>SolutionPackagerRelativePath</t>
+  </si>
+  <si>
+    <t>CoreTools\solutionpackager.exe</t>
+  </si>
+  <si>
+    <t>SolutionToBeImported</t>
+  </si>
+  <si>
+    <t>DD365\SolutionToBeImported.ps1</t>
+  </si>
+  <si>
+    <t>SoulutionCheckerConfigFile</t>
+  </si>
+  <si>
+    <t>TriggerFile</t>
+  </si>
+  <si>
+    <t>source\html</t>
+  </si>
+  <si>
+    <t>source\images</t>
+  </si>
+  <si>
+    <t>source\js</t>
+  </si>
+  <si>
+    <t>Test\Release</t>
+  </si>
+  <si>
+    <t>DD365\CheckIn</t>
+  </si>
+  <si>
+    <t>DD365\Release</t>
+  </si>
 </sst>
 </file>
 
@@ -313,7 +416,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,6 +432,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,7 +490,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -415,6 +524,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -902,7 +1017,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -969,12 +1084,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45">
+    <row r="5" spans="1:4" ht="30">
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>35</v>
+      <c r="B5" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>22</v>
@@ -1143,8 +1258,181 @@
     <hyperlink ref="B7" r:id="rId2" xr:uid="{91C77408-B28A-40E7-A1EE-C60B68E6F57E}"/>
     <hyperlink ref="B11" r:id="rId3" xr:uid="{2F5516A2-37EE-4E2C-A43D-63575578D21E}"/>
     <hyperlink ref="B9" r:id="rId4" xr:uid="{F6C101D5-7FE4-4923-B8F6-36E818F78B85}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{EF94B173-F6B5-4D93-8C72-5B4CA7FC5632}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA44A09-FB88-462E-A9D9-8257E778990C}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="15">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>